<commit_message>
a bunch of updates
</commit_message>
<xml_diff>
--- a/data/california/proposed_expansion/CDFW_2020_proposed_biotoxin_zones_sites.xlsx
+++ b/data/california/proposed_expansion/CDFW_2020_proposed_biotoxin_zones_sites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/domoic_acid_mgmt/data/california/proposed_expansion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138ADFE2-6D75-0546-BFD4-7ED51A9C6EFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE322571-8F49-A249-9293-1795A62991B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5080" yWindow="6560" windowWidth="15000" windowHeight="16460" activeTab="1" xr2:uid="{6529BC81-5A96-A246-8FEB-6C5E101FDDFD}"/>
+    <workbookView xWindow="5080" yWindow="6560" windowWidth="15000" windowHeight="16460" xr2:uid="{6529BC81-5A96-A246-8FEB-6C5E101FDDFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sites" sheetId="1" r:id="rId1"/>
@@ -214,9 +214,6 @@
     <t>42°</t>
   </si>
   <si>
-    <t>Pillar Point (Half Moon Bay?)</t>
-  </si>
-  <si>
     <t>new</t>
   </si>
   <si>
@@ -236,6 +233,9 @@
   </si>
   <si>
     <t>CA/Mexicio Border</t>
+  </si>
+  <si>
+    <t>Pillar Point (Half Moon Bay)</t>
   </si>
 </sst>
 </file>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30080DA-12BA-844A-A174-99746358C64B}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,7 +660,7 @@
         <v>40</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -686,7 +686,7 @@
         <v>-124.25</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -712,7 +712,7 @@
         <v>-124.183333333333</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -738,7 +738,7 @@
         <v>-124.15</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -764,7 +764,7 @@
         <v>-124.15</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -790,7 +790,7 @@
         <v>-124.23333333333299</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -816,7 +816,7 @@
         <v>-124.383333333333</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -833,7 +833,7 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F8" s="4">
         <v>39.799999999999997</v>
@@ -842,7 +842,7 @@
         <v>-123.883333333333</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -859,7 +859,7 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F9" s="4">
         <v>38.974645000000002</v>
@@ -868,10 +868,10 @@
         <v>-123.743331</v>
       </c>
       <c r="H9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" t="s">
         <v>67</v>
-      </c>
-      <c r="I9" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -888,7 +888,7 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" s="4">
         <v>38.567892000000001</v>
@@ -897,10 +897,10 @@
         <v>-123.378792</v>
       </c>
       <c r="H10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" t="s">
         <v>67</v>
-      </c>
-      <c r="I10" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -926,7 +926,7 @@
         <v>-123.183333333333</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -943,7 +943,7 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F12" s="4">
         <v>38.295214000000001</v>
@@ -952,10 +952,10 @@
         <v>-123.07026</v>
       </c>
       <c r="H12" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12" t="s">
         <v>67</v>
-      </c>
-      <c r="I12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -981,7 +981,7 @@
         <v>-123.05</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1007,7 +1007,7 @@
         <v>-122.76666666666701</v>
       </c>
       <c r="H14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1021,7 +1021,7 @@
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>42</v>
@@ -1033,10 +1033,10 @@
         <v>-122.683333333333</v>
       </c>
       <c r="H15" t="s">
+        <v>64</v>
+      </c>
+      <c r="I15" t="s">
         <v>65</v>
-      </c>
-      <c r="I15" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1053,7 +1053,7 @@
         <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F16" s="4">
         <v>37.185983</v>
@@ -1062,10 +1062,10 @@
         <v>-122.426063</v>
       </c>
       <c r="H16" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16" t="s">
         <v>67</v>
-      </c>
-      <c r="I16" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1082,7 +1082,7 @@
         <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" s="4">
         <v>36.645954000000003</v>
@@ -1091,10 +1091,10 @@
         <v>-121.883115</v>
       </c>
       <c r="H17" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17" t="s">
         <v>67</v>
-      </c>
-      <c r="I17" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1111,7 +1111,7 @@
         <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" s="4">
         <v>35.128770000000003</v>
@@ -1120,10 +1120,10 @@
         <v>-120.74531399999999</v>
       </c>
       <c r="H18" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" t="s">
         <v>67</v>
-      </c>
-      <c r="I18" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1139,7 +1139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C09F644-840E-E64B-818E-1736750990F9}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1267,7 +1267,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="5">
         <v>32.534343</v>

</xml_diff>